<commit_message>
Modified UniversityDatabase. Added ClientView page where users can view bookings.
</commit_message>
<xml_diff>
--- a/src/database/UniversityDatabase.xlsx
+++ b/src/database/UniversityDatabase.xlsx
@@ -5,17 +5,15 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sheida\engineering\year 3\winter\eecs3311\eecs3311\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sheid\git\YorkUParkingBookingSystem\src\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BFDAC68-3331-4FE0-AD6C-7D72663C321F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886392C1-1C23-437C-A27B-38B81EDED16F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{7C63F0BD-F4E4-4DA5-9E8C-0B2055B64285}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7C63F0BD-F4E4-4DA5-9E8C-0B2055B64285}"/>
   </bookViews>
   <sheets>
-    <sheet name="FacultyMembers" sheetId="2" r:id="rId1"/>
-    <sheet name="Students" sheetId="1" r:id="rId2"/>
-    <sheet name="NonFacultyStaff" sheetId="3" r:id="rId3"/>
+    <sheet name="UniversityMembers" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Email</t>
   </si>
@@ -92,6 +90,18 @@
   </si>
   <si>
     <t>natalie@my.yorku.ca</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>FacultyMember</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>NonFacultyStaff</t>
   </si>
 </sst>
 </file>
@@ -483,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{478439A2-9358-4243-AB31-25FF76B9D451}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -495,148 +505,116 @@
     <col min="2" max="2" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{6C135CEA-8F29-4DF4-BDFD-51B5C00D05F3}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{6B446A1A-8445-4C08-8AFB-35AE406F16C5}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{618A6925-C59D-48D8-AAFD-43C4F6869B40}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{9C78FF9D-DA80-494F-A003-380E772E21B6}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{9C9B4C07-944D-4DA0-9AA4-3D7FE77D1F79}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{40FF9611-C3C0-48D6-8C75-0E07A22F4D90}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{C4BFF46F-F87B-42B1-8457-7F1CE629AC94}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{78EAF1FA-8632-47B5-86E6-4C3277187528}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B44D5AC8-B0B5-4788-A5AC-91916F520FA0}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="22.109375" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{8A6E7C6E-34D9-4D6F-9F29-1A239032EA0E}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{14A173CC-F7EA-4240-A7AE-5D0AF165743F}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{B9171A86-3D1D-410D-A99A-104A07051B0E}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{4B7BAB46-632F-43E4-9E56-4757127D3AFE}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D50B07A-82DA-4994-9EB2-4662E00D92C3}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="11.21875" customWidth="1"/>
-    <col min="2" max="2" width="18.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{5BA26FF8-6B62-4E8C-868D-D13AAE7F1DE2}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{D3F451E7-7DE1-4B9C-86DC-5D86B06700F0}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
-</worksheet>
 </file>
</xml_diff>